<commit_message>
Change TIM4 to TIM3
</commit_message>
<xml_diff>
--- a/Garbage-Disposer-Controller/Doc/IO.xlsx
+++ b/Garbage-Disposer-Controller/Doc/IO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14688" windowHeight="13595"/>
+    <workbookView windowWidth="30048" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t>PC6</t>
   </si>
@@ -130,7 +130,19 @@
     <t>TIM2-CH4</t>
   </si>
   <si>
-    <t>PB6</t>
+    <r>
+      <t xml:space="preserve">PB6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PB4</t>
+    </r>
   </si>
   <si>
     <t>PWM_Step_Fenli_L</t>
@@ -139,7 +151,22 @@
     <t>TIM4-CH1</t>
   </si>
   <si>
-    <t>PB7</t>
+    <t>TIM3-CH1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PB7 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PB5</t>
+    </r>
   </si>
   <si>
     <t>PWM_Step_Fenli_R</t>
@@ -148,7 +175,22 @@
     <t>TIM4-CH2</t>
   </si>
   <si>
-    <t>PB8</t>
+    <t>TIM3-CH2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PB8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PB0</t>
+    </r>
   </si>
   <si>
     <t>PWM_Step_Dian</t>
@@ -157,10 +199,28 @@
     <t>TIM4-CH3</t>
   </si>
   <si>
-    <t>PB9</t>
+    <t>TIM3-CH3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PB9 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PB1</t>
+    </r>
   </si>
   <si>
     <t>TIM4-CH4</t>
+  </si>
+  <si>
+    <t>TIM3-CH4</t>
   </si>
   <si>
     <t>PD0</t>
@@ -217,11 +277,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,11 +293,25 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -246,12 +320,42 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,8 +364,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,59 +403,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -336,9 +411,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -346,29 +421,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,187 +450,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,37 +644,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,6 +700,26 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -651,26 +727,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -682,10 +749,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -694,138 +761,144 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1147,13 +1220,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="9.77777777777778" customWidth="1"/>
@@ -1320,8 +1393,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
@@ -1330,43 +1403,55 @@
       <c r="C20" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+      <c r="D20" s="2" t="s">
         <v>41</v>
       </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
         <v>44</v>
       </c>
+      <c r="D21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
@@ -1374,10 +1459,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
@@ -1385,10 +1470,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
@@ -1396,51 +1481,51 @@
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
         <v>62</v>
-      </c>
-      <c r="C32" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>